<commit_message>
feat: init ai comment analysis
</commit_message>
<xml_diff>
--- a/backend/core/agents/comments.xlsx
+++ b/backend/core/agents/comments.xlsx
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
-  <si>
-    <t>comment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>1. Yesss you’re doing this so right</t>
   </si>
@@ -1510,10 +1507,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A113"/>
+  <dimension ref="A1:A112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A$1:A$1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.234375" defaultRowHeight="16.8"/>
@@ -2081,11 +2078,6 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
-      <c r="A113" t="s">
-        <v>112</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>